<commit_message>
geração de histogramas para aon, flex e sub nas dimensões total, meta e contrib
</commit_message>
<xml_diff>
--- a/analises/2023/analise_descritiva/dados/panorama.xlsx
+++ b/analises/2023/analise_descritiva/dados/panorama.xlsx
@@ -757,10 +757,10 @@
         <v>165199.0578149446</v>
       </c>
       <c r="G4" s="3">
-        <v>1205.832538795216</v>
+        <v>1086.835906677267</v>
       </c>
       <c r="H4" s="3">
-        <v>2163.288658625352</v>
+        <v>2084.495516178294</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>

</xml_diff>